<commit_message>
add some dates to wziardry
</commit_message>
<xml_diff>
--- a/wizardry/checklist.xlsx
+++ b/wizardry/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/wizardry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1803D2-9C82-A94D-BAB3-DAA1841C1D73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C73E5E-8AA9-A147-BBAA-45F7A0DE8F69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{A10FCA2F-080B-F24A-BFED-6A5E85894061}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{A10FCA2F-080B-F24A-BFED-6A5E85894061}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AE3480F-D3C2-5B4A-BCA4-BABFD1667664}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,6 +678,9 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1989</v>
+      </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -695,6 +698,9 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1989</v>
+      </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
@@ -712,6 +718,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1989</v>
+      </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
@@ -729,6 +738,9 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1990</v>
+      </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>

</xml_diff>